<commit_message>
update for spi dma support.
</commit_message>
<xml_diff>
--- a/Document/设计文档.xlsx
+++ b/Document/设计文档.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\GitProgram\STM32_Handler\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF31AF3-9C28-4013-B669-FEE65DC017E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46655E76-7F0C-44C9-AA18-4C471E9AF6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="122">
   <si>
     <t>外部引脚</t>
   </si>
@@ -203,212 +203,220 @@
     <t>Nand FLASH</t>
   </si>
   <si>
+    <t>串口IAP实验</t>
+  </si>
+  <si>
+    <t>IAP</t>
+  </si>
+  <si>
+    <t>rtos</t>
+  </si>
+  <si>
+    <t>单片机硬件</t>
+  </si>
+  <si>
+    <t>窗口看门狗</t>
+  </si>
+  <si>
+    <t>WWDG</t>
+  </si>
+  <si>
+    <t>TFTLCD(RGB屏)</t>
+  </si>
+  <si>
+    <t>LTDC</t>
+  </si>
+  <si>
+    <t>USMART调试组件</t>
+  </si>
+  <si>
+    <t>OLED显示</t>
+  </si>
+  <si>
+    <t>并口IO模拟</t>
+  </si>
+  <si>
+    <t>UART+RS485</t>
+  </si>
+  <si>
+    <t>DS18B20</t>
+  </si>
+  <si>
+    <t>I/O</t>
+  </si>
+  <si>
+    <t>DH11数字湿度传感器</t>
+  </si>
+  <si>
+    <t>无线通讯</t>
+  </si>
+  <si>
+    <t>SPI+NRF24L01</t>
+  </si>
+  <si>
+    <t>摄像头</t>
+  </si>
+  <si>
+    <t>DCMI</t>
+  </si>
+  <si>
+    <t>内存管理</t>
+  </si>
+  <si>
+    <t>malloc/free</t>
+  </si>
+  <si>
+    <t>照相机</t>
+  </si>
+  <si>
+    <t>视频播放</t>
+  </si>
+  <si>
+    <t>Mege</t>
+  </si>
+  <si>
+    <t>手写识别</t>
+  </si>
+  <si>
+    <t>T9拼音输入法</t>
+  </si>
+  <si>
+    <t>USB读卡器(Slave)</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>USB声卡(Slave)</t>
+  </si>
+  <si>
+    <t>红外遥控</t>
+  </si>
+  <si>
+    <t>Timer Capture</t>
+  </si>
+  <si>
+    <t>FLASH存储管理方案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图片显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图像处理库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>界面管理实现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stemwin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SDIO，FATFS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字库处理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FMC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FreeRTOS相关应用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB应用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ETH，LWIP，HTTTP，SNMP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>虚拟串口，U盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低功耗实现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>待机唤醒，休眠管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>音乐输出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W25Q256，触摸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I2C接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCF8574，AP3216c, mpu9250</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>录音机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FLASH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SD卡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>汉字显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>网络通讯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB鼠标键盘(Host)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>FPU测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>fpu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DSP测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>dsp</t>
-  </si>
-  <si>
-    <t>串口IAP实验</t>
-  </si>
-  <si>
-    <t>IAP</t>
-  </si>
-  <si>
-    <t>rtos</t>
-  </si>
-  <si>
-    <t>单片机硬件</t>
-  </si>
-  <si>
-    <t>窗口看门狗</t>
-  </si>
-  <si>
-    <t>WWDG</t>
-  </si>
-  <si>
-    <t>TFTLCD(RGB屏)</t>
-  </si>
-  <si>
-    <t>LTDC</t>
-  </si>
-  <si>
-    <t>USMART调试组件</t>
-  </si>
-  <si>
-    <t>OLED显示</t>
-  </si>
-  <si>
-    <t>并口IO模拟</t>
-  </si>
-  <si>
-    <t>UART+RS485</t>
-  </si>
-  <si>
-    <t>DS18B20</t>
-  </si>
-  <si>
-    <t>I/O</t>
-  </si>
-  <si>
-    <t>DH11数字湿度传感器</t>
-  </si>
-  <si>
-    <t>无线通讯</t>
-  </si>
-  <si>
-    <t>SPI+NRF24L01</t>
-  </si>
-  <si>
-    <t>摄像头</t>
-  </si>
-  <si>
-    <t>DCMI</t>
-  </si>
-  <si>
-    <t>内存管理</t>
-  </si>
-  <si>
-    <t>malloc/free</t>
-  </si>
-  <si>
-    <t>照相机</t>
-  </si>
-  <si>
-    <t>视频播放</t>
-  </si>
-  <si>
-    <t>Mege</t>
-  </si>
-  <si>
-    <t>手写识别</t>
-  </si>
-  <si>
-    <t>T9拼音输入法</t>
-  </si>
-  <si>
-    <t>USB读卡器(Slave)</t>
-  </si>
-  <si>
-    <t>USB</t>
-  </si>
-  <si>
-    <t>USB声卡(Slave)</t>
-  </si>
-  <si>
-    <t>红外遥控</t>
-  </si>
-  <si>
-    <t>Timer Capture</t>
-  </si>
-  <si>
-    <t>FLASH存储管理方案</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>图片显示</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>图像处理库</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>界面管理实现</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stemwin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SDIO，FATFS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>字库处理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FMC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FreeRTOS相关应用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>USB应用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ETH，LWIP，HTTTP，SNMP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>虚拟串口，U盘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>低功耗实现</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>待机唤醒，休眠管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>音乐输出</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>W25Q256，触摸</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>I2C接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PCF8574，AP3216c, mpu9250</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>To do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>录音机</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FLASH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SD卡</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>汉字显示</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>网络通讯</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SAI+WM8978</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>USB鼠标键盘(Host)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SAI+WM8978，音频处理</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -546,15 +554,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -571,6 +570,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -937,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40:D52"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -956,11 +964,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -977,13 +985,13 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="8" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -991,13 +999,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="8" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -1005,13 +1013,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1019,333 +1027,333 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="11" t="s">
+      <c r="A8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="C21" s="11" t="s">
+      <c r="A21" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A22" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="11" t="s">
+      <c r="A22" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A23" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>28</v>
+      <c r="A23" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A24" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>28</v>
+      <c r="A24" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="18" t="s">
-        <v>110</v>
+      <c r="B25" s="15" t="s">
+        <v>106</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A27" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>119</v>
+        <v>105</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>121</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>121</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="7" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
@@ -1353,7 +1361,7 @@
         <v>59</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>28</v>
@@ -1361,10 +1369,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>28</v>
@@ -1372,10 +1380,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>28</v>
@@ -1383,7 +1391,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>20</v>
@@ -1394,139 +1402,139 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="17"/>
+      <c r="D41" s="14"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D42" s="16"/>
+      <c r="D42" s="13"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D43" s="17"/>
+      <c r="D43" s="14"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="6">
         <v>485</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D44" s="17"/>
+      <c r="D44" s="14"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D45" s="17"/>
+      <c r="D45" s="14"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D46" s="17"/>
+      <c r="D46" s="14"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="17"/>
+      <c r="D47" s="14"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D48" s="17"/>
+      <c r="D48" s="14"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D49" s="17"/>
+      <c r="D49" s="14"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D50" s="17"/>
+      <c r="D50" s="14"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D51" s="17"/>
+      <c r="D51" s="14"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>31</v>
@@ -1534,7 +1542,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>31</v>
@@ -1542,7 +1550,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>31</v>
@@ -1550,10 +1558,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>31</v>
@@ -1561,21 +1569,21 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="16" t="s">
-        <v>120</v>
+      <c r="A57" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>31</v>
@@ -1587,7 +1595,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C38" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C31:C38 C3:C30" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$F$2:$F$5</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
support timer extend clock.
</commit_message>
<xml_diff>
--- a/Document/设计文档.xlsx
+++ b/Document/设计文档.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\GitProgram\STM32_Handler\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46655E76-7F0C-44C9-AA18-4C471E9AF6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80DF53B-37A1-4799-AB3E-C13CAE1A6261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -170,253 +170,254 @@
     <t>RTC</t>
   </si>
   <si>
+    <t>硬件随机数</t>
+  </si>
+  <si>
+    <t>RNG</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>内部温度传感器</t>
+  </si>
+  <si>
+    <t>ADC+Convert</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
+    <t>DAC</t>
+  </si>
+  <si>
+    <t>DMA</t>
+  </si>
+  <si>
+    <t>CAN通讯</t>
+  </si>
+  <si>
+    <t>Nand FLASH</t>
+  </si>
+  <si>
+    <t>串口IAP实验</t>
+  </si>
+  <si>
+    <t>IAP</t>
+  </si>
+  <si>
+    <t>rtos</t>
+  </si>
+  <si>
+    <t>单片机硬件</t>
+  </si>
+  <si>
+    <t>窗口看门狗</t>
+  </si>
+  <si>
+    <t>WWDG</t>
+  </si>
+  <si>
+    <t>TFTLCD(RGB屏)</t>
+  </si>
+  <si>
+    <t>LTDC</t>
+  </si>
+  <si>
+    <t>USMART调试组件</t>
+  </si>
+  <si>
+    <t>OLED显示</t>
+  </si>
+  <si>
+    <t>并口IO模拟</t>
+  </si>
+  <si>
+    <t>UART+RS485</t>
+  </si>
+  <si>
+    <t>DS18B20</t>
+  </si>
+  <si>
+    <t>I/O</t>
+  </si>
+  <si>
+    <t>DH11数字湿度传感器</t>
+  </si>
+  <si>
+    <t>无线通讯</t>
+  </si>
+  <si>
+    <t>SPI+NRF24L01</t>
+  </si>
+  <si>
+    <t>摄像头</t>
+  </si>
+  <si>
+    <t>DCMI</t>
+  </si>
+  <si>
+    <t>内存管理</t>
+  </si>
+  <si>
+    <t>malloc/free</t>
+  </si>
+  <si>
+    <t>照相机</t>
+  </si>
+  <si>
+    <t>视频播放</t>
+  </si>
+  <si>
+    <t>Mege</t>
+  </si>
+  <si>
+    <t>手写识别</t>
+  </si>
+  <si>
+    <t>T9拼音输入法</t>
+  </si>
+  <si>
+    <t>USB读卡器(Slave)</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>USB声卡(Slave)</t>
+  </si>
+  <si>
+    <t>红外遥控</t>
+  </si>
+  <si>
+    <t>Timer Capture</t>
+  </si>
+  <si>
+    <t>FLASH存储管理方案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图片显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图像处理库</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>界面管理实现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stemwin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SDIO，FATFS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字库处理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FMC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FreeRTOS相关应用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB应用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ETH，LWIP，HTTTP，SNMP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>虚拟串口，U盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>低功耗实现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>待机唤醒，休眠管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>音乐输出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W25Q256，触摸</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I2C接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCF8574，AP3216c, mpu9250</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>To do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>录音机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FLASH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SD卡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>汉字显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>网络通讯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB鼠标键盘(Host)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FPU测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fpu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DSP测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dsp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SAI+WM8978，音频处理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>SPI</t>
-  </si>
-  <si>
-    <t>硬件随机数</t>
-  </si>
-  <si>
-    <t>RNG</t>
-  </si>
-  <si>
-    <t>ADC</t>
-  </si>
-  <si>
-    <t>内部温度传感器</t>
-  </si>
-  <si>
-    <t>ADC+Convert</t>
-  </si>
-  <si>
-    <t>CAN</t>
-  </si>
-  <si>
-    <t>DAC</t>
-  </si>
-  <si>
-    <t>DMA</t>
-  </si>
-  <si>
-    <t>CAN通讯</t>
-  </si>
-  <si>
-    <t>Nand FLASH</t>
-  </si>
-  <si>
-    <t>串口IAP实验</t>
-  </si>
-  <si>
-    <t>IAP</t>
-  </si>
-  <si>
-    <t>rtos</t>
-  </si>
-  <si>
-    <t>单片机硬件</t>
-  </si>
-  <si>
-    <t>窗口看门狗</t>
-  </si>
-  <si>
-    <t>WWDG</t>
-  </si>
-  <si>
-    <t>TFTLCD(RGB屏)</t>
-  </si>
-  <si>
-    <t>LTDC</t>
-  </si>
-  <si>
-    <t>USMART调试组件</t>
-  </si>
-  <si>
-    <t>OLED显示</t>
-  </si>
-  <si>
-    <t>并口IO模拟</t>
-  </si>
-  <si>
-    <t>UART+RS485</t>
-  </si>
-  <si>
-    <t>DS18B20</t>
-  </si>
-  <si>
-    <t>I/O</t>
-  </si>
-  <si>
-    <t>DH11数字湿度传感器</t>
-  </si>
-  <si>
-    <t>无线通讯</t>
-  </si>
-  <si>
-    <t>SPI+NRF24L01</t>
-  </si>
-  <si>
-    <t>摄像头</t>
-  </si>
-  <si>
-    <t>DCMI</t>
-  </si>
-  <si>
-    <t>内存管理</t>
-  </si>
-  <si>
-    <t>malloc/free</t>
-  </si>
-  <si>
-    <t>照相机</t>
-  </si>
-  <si>
-    <t>视频播放</t>
-  </si>
-  <si>
-    <t>Mege</t>
-  </si>
-  <si>
-    <t>手写识别</t>
-  </si>
-  <si>
-    <t>T9拼音输入法</t>
-  </si>
-  <si>
-    <t>USB读卡器(Slave)</t>
-  </si>
-  <si>
-    <t>USB</t>
-  </si>
-  <si>
-    <t>USB声卡(Slave)</t>
-  </si>
-  <si>
-    <t>红外遥控</t>
-  </si>
-  <si>
-    <t>Timer Capture</t>
-  </si>
-  <si>
-    <t>FLASH存储管理方案</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>图片显示</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>图像处理库</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>界面管理实现</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stemwin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SDIO，FATFS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>字库处理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FMC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FreeRTOS相关应用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>USB应用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ETH，LWIP，HTTTP，SNMP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>虚拟串口，U盘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>低功耗实现</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>待机唤醒，休眠管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>音乐输出</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>W25Q256，触摸</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>I2C接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PCF8574，AP3216c, mpu9250</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>To do</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>录音机</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FLASH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SD卡</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>汉字显示</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>网络通讯</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>USB鼠标键盘(Host)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FPU测试</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fpu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Complete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DSP测试</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dsp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SAI+WM8978，音频处理</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -533,7 +534,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -567,7 +568,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -946,7 +946,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -964,11 +964,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -1050,10 +1050,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>65</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>22</v>
@@ -1138,10 +1138,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>51</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>22</v>
@@ -1149,10 +1149,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>22</v>
@@ -1160,10 +1160,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>22</v>
@@ -1171,10 +1171,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>22</v>
@@ -1182,21 +1182,21 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="15" t="s">
         <v>107</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>108</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>22</v>
@@ -1204,10 +1204,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>22</v>
@@ -1215,54 +1215,54 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="C23" s="10" t="s">
         <v>117</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>120</v>
-      </c>
       <c r="C24" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A25" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>28</v>
+      <c r="A25" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>109</v>
+      <c r="A26" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>28</v>
@@ -1270,98 +1270,98 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>109</v>
+      <c r="C30" s="10" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>93</v>
-      </c>
       <c r="C32" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="C33" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>28</v>
@@ -1369,10 +1369,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>28</v>
@@ -1380,10 +1380,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>28</v>
@@ -1391,7 +1391,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>20</v>
@@ -1402,10 +1402,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>31</v>
@@ -1414,7 +1414,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>31</v>
@@ -1423,10 +1423,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>31</v>
@@ -1438,7 +1438,7 @@
         <v>485</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>31</v>
@@ -1447,10 +1447,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>31</v>
@@ -1459,10 +1459,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>31</v>
@@ -1471,10 +1471,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>31</v>
@@ -1483,10 +1483,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>31</v>
@@ -1495,10 +1495,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>31</v>
@@ -1507,10 +1507,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>31</v>
@@ -1519,10 +1519,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>31</v>
@@ -1531,10 +1531,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>31</v>
@@ -1542,7 +1542,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>31</v>
@@ -1550,7 +1550,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>31</v>
@@ -1558,10 +1558,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>31</v>
@@ -1569,10 +1569,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>31</v>
@@ -1580,10 +1580,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>31</v>

</xml_diff>